<commit_message>
Created final Python files
</commit_message>
<xml_diff>
--- a/project1/runs/cqr/CQR_Analysis.xlsx
+++ b/project1/runs/cqr/CQR_Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\Desktop\Coding\MATH-505\project1\runs\cqr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE50DCB-FDD3-4AAB-A8DC-ABDB8AB4AC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BB5C80-5B8D-4B8F-8577-D11BCA0FA788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{96ABD8B0-1B3A-4FB5-B8A8-89003737A69A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{96ABD8B0-1B3A-4FB5-B8A8-89003737A69A}"/>
   </bookViews>
   <sheets>
     <sheet name="cqr_results" sheetId="2" r:id="rId1"/>
@@ -114,8 +114,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1544,7 +1545,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1830,6 +1830,839 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>CQR Condition Number of Q vs A</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$G$1:$G$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="72"/>
+                <c:pt idx="0">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.31</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.51</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.62</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.69</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.08</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.1800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.4900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.5499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.61</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.79</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.97</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.12</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.18</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.24</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.79</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.84</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.04</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.17</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.18</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.1900000000000004</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.33</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.34</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.4800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.72</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.8099999999999996</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.8499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.05</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.09</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.15</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.23</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.32</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.37</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5.37</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.39</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5.39</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5.62</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5.79</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5.99</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>6.26</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6.53</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>6.59</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>6.67</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>6.69</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>6.69</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>7.27</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>7.48</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>7.53</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>7.54</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>7.56</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>7.62</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>7.77</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>7.84</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>7.93</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>8.09</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>8.2799999999999994</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>8.32</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>8.43</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$1:$H$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="72"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.03</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.1299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.26</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.73</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.52</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-480A-4C7A-96A4-FA507146D173}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="353891007"/>
+        <c:axId val="463395855"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="353891007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Condition Number of A (Log10 Scale)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="463395855"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="463395855"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2.6"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Condition Number of Q</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="353891007"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1871,6 +2704,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2942,6 +3815,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3010,6 +4399,47 @@
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>72389</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>286342</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>42312</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4578799-53A9-14A6-B482-36651719A487}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -6342,7 +7772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0660C32-C6DB-4B51-9C34-C548AA9A2C56}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -6521,13 +7951,1820 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93D6459-445F-4323-B042-1CDBD5E680EF}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="124" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>0.20247459000000001</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1.94130392367618E-13</v>
+      </c>
+      <c r="C1">
+        <v>3.2164411645697402</v>
+      </c>
+      <c r="D1" s="1">
+        <v>1.4101064053820899E-15</v>
+      </c>
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="G1">
+        <f>ROUND(LOG10(C1),2)</f>
+        <v>0.51</v>
+      </c>
+      <c r="H1">
+        <f>ROUND(E1,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0.20804204600000001</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2.6307051745991299E-13</v>
+      </c>
+      <c r="C2">
+        <v>4.4727236449661598</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2.1253217854725601E-15</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:G65" si="0">ROUND(LOG10(C2),2)</f>
+        <v>0.65</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ref="H2:H65" si="1">ROUND(E2,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0.19879465099999999</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3.3570696783024201E-13</v>
+      </c>
+      <c r="C3">
+        <v>8.5282582554314903</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3.32734140912611E-15</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>0.93</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0.178173361</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4.13916050866269E-13</v>
+      </c>
+      <c r="C4">
+        <v>11.9782962357695</v>
+      </c>
+      <c r="D4" s="1">
+        <v>6.1162433676951302E-15</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>1.08</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0.20014216900000001</v>
+      </c>
+      <c r="B5" s="1">
+        <v>6.4236150698248203E-13</v>
+      </c>
+      <c r="C5">
+        <v>19.392046288318099</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.46102993724651E-14</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>1.29</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0.196177301</v>
+      </c>
+      <c r="B6" s="1">
+        <v>6.9832245732141003E-13</v>
+      </c>
+      <c r="C6">
+        <v>20.455520216018801</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.9224102167616899E-14</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>1.31</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0.20237454199999999</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4.6078276365394398E-13</v>
+      </c>
+      <c r="C7">
+        <v>32.270760290459002</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3.1287193991197699E-14</v>
+      </c>
+      <c r="E7">
+        <v>1.00000000000001</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>1.51</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0.22330831700000001</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.13871359055383E-12</v>
+      </c>
+      <c r="C8">
+        <v>41.4710403851536</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5.7371015858288894E-14</v>
+      </c>
+      <c r="E8">
+        <v>1.00000000000001</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>1.62</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0.20516336800000001</v>
+      </c>
+      <c r="B9" s="1">
+        <v>7.6519192391921602E-13</v>
+      </c>
+      <c r="C9">
+        <v>48.651909048172698</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1.05701941188613E-13</v>
+      </c>
+      <c r="E9">
+        <v>1.00000000000005</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>1.69</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0.20306687300000001</v>
+      </c>
+      <c r="B10" s="1">
+        <v>9.2234158642730305E-13</v>
+      </c>
+      <c r="C10">
+        <v>121.56273816888999</v>
+      </c>
+      <c r="D10" s="1">
+        <v>8.7579335654524104E-13</v>
+      </c>
+      <c r="E10">
+        <v>1.0000000000004401</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>2.08</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0.21213411699999901</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.94156547267682E-12</v>
+      </c>
+      <c r="C11">
+        <v>134.67058248594699</v>
+      </c>
+      <c r="D11" s="1">
+        <v>4.7346492623578098E-13</v>
+      </c>
+      <c r="E11">
+        <v>1.00000000000027</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>2.13</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0.200557069</v>
+      </c>
+      <c r="B12" s="1">
+        <v>6.8739830062005902E-13</v>
+      </c>
+      <c r="C12">
+        <v>151.209407103052</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1.40704130458115E-12</v>
+      </c>
+      <c r="E12">
+        <v>1.00000000000078</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0.21941438199999999</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.4197463069337401E-12</v>
+      </c>
+      <c r="C13">
+        <v>157.48021248196099</v>
+      </c>
+      <c r="D13" s="1">
+        <v>6.0588292963300601E-13</v>
+      </c>
+      <c r="E13">
+        <v>1.00000000000032</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0.21030348500000001</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.78063407316235E-12</v>
+      </c>
+      <c r="C14">
+        <v>309.24172803163401</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2.6664888473138299E-12</v>
+      </c>
+      <c r="E14">
+        <v>1.0000000000015901</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0.204305021</v>
+      </c>
+      <c r="B15" s="1">
+        <v>5.2377781878961897E-12</v>
+      </c>
+      <c r="C15">
+        <v>355.72883222356597</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3.98776455029945E-12</v>
+      </c>
+      <c r="E15">
+        <v>1.0000000000020499</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0.21377458399999999</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.67158644585764E-12</v>
+      </c>
+      <c r="C16">
+        <v>411.653612574921</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3.8836848253647703E-12</v>
+      </c>
+      <c r="E16">
+        <v>1.00000000000191</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>2.61</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0.20010671899999999</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2.3363648963588301E-12</v>
+      </c>
+      <c r="C17">
+        <v>611.01684024829501</v>
+      </c>
+      <c r="D17" s="1">
+        <v>7.1172967102871304E-12</v>
+      </c>
+      <c r="E17">
+        <v>1.0000000000043701</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>2.79</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0.182877593</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.5429705915403201E-12</v>
+      </c>
+      <c r="C18">
+        <v>637.19497365089796</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1.1720876247802E-11</v>
+      </c>
+      <c r="E18">
+        <v>1.00000000000697</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>2.8</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0.22686599799999899</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2.6130288853094201E-12</v>
+      </c>
+      <c r="C19">
+        <v>926.27551865747705</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2.9295425551997999E-11</v>
+      </c>
+      <c r="E19">
+        <v>1.0000000000157001</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>2.97</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0.22026659600000001</v>
+      </c>
+      <c r="B20" s="1">
+        <v>7.20144832557301E-12</v>
+      </c>
+      <c r="C20">
+        <v>1328.42536131365</v>
+      </c>
+      <c r="D20" s="1">
+        <v>3.8284146429334201E-11</v>
+      </c>
+      <c r="E20">
+        <v>1.0000000000220199</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>3.12</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0.226168537</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2.4184790638040901E-12</v>
+      </c>
+      <c r="C21">
+        <v>1503.4031564076299</v>
+      </c>
+      <c r="D21" s="1">
+        <v>5.5892219032101602E-11</v>
+      </c>
+      <c r="E21">
+        <v>1.0000000000318201</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>3.18</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>0.24459081799999999</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2.1591752759410999E-12</v>
+      </c>
+      <c r="C22">
+        <v>1749.5086582232</v>
+      </c>
+      <c r="D22" s="1">
+        <v>7.2612297195371398E-11</v>
+      </c>
+      <c r="E22">
+        <v>1.00000000004135</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>3.24</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>0.22228547900000001</v>
+      </c>
+      <c r="B23" s="1">
+        <v>3.2099571093907001E-12</v>
+      </c>
+      <c r="C23">
+        <v>6156.4712185572598</v>
+      </c>
+      <c r="D23" s="1">
+        <v>6.0091851896270595E-10</v>
+      </c>
+      <c r="E23">
+        <v>1.00000000030915</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>3.79</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>0.216419995999999</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.7012986979964099E-11</v>
+      </c>
+      <c r="C24">
+        <v>6896.2236151366596</v>
+      </c>
+      <c r="D24" s="1">
+        <v>7.4510116163962701E-10</v>
+      </c>
+      <c r="E24">
+        <v>1.00000000043338</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>3.84</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>0.223406258</v>
+      </c>
+      <c r="B25" s="1">
+        <v>4.3021271706872499E-12</v>
+      </c>
+      <c r="C25">
+        <v>10946.233962336901</v>
+      </c>
+      <c r="D25" s="1">
+        <v>3.4213699171682098E-9</v>
+      </c>
+      <c r="E25">
+        <v>1.0000000019145701</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>4.04</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>0.22900216600000001</v>
+      </c>
+      <c r="B26" s="1">
+        <v>3.3062645872484902E-12</v>
+      </c>
+      <c r="C26">
+        <v>14712.773232899901</v>
+      </c>
+      <c r="D26" s="1">
+        <v>4.87017765562776E-9</v>
+      </c>
+      <c r="E26">
+        <v>1.0000000024420601</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>4.17</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>0.22066954699999999</v>
+      </c>
+      <c r="B27" s="1">
+        <v>9.3910188452138403E-11</v>
+      </c>
+      <c r="C27">
+        <v>15155.886824339001</v>
+      </c>
+      <c r="D27" s="1">
+        <v>4.3461739872849201E-9</v>
+      </c>
+      <c r="E27">
+        <v>1.00000000297836</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>4.18</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0.245559005</v>
+      </c>
+      <c r="B28" s="1">
+        <v>5.2960979557890098E-12</v>
+      </c>
+      <c r="C28">
+        <v>15658.830651246801</v>
+      </c>
+      <c r="D28" s="1">
+        <v>3.2626599198179198E-9</v>
+      </c>
+      <c r="E28">
+        <v>1.0000000017303301</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>0.24966461100000001</v>
+      </c>
+      <c r="B29" s="1">
+        <v>3.7547616899426298E-12</v>
+      </c>
+      <c r="C29">
+        <v>21619.369756484801</v>
+      </c>
+      <c r="D29" s="1">
+        <v>5.7693079620071602E-9</v>
+      </c>
+      <c r="E29">
+        <v>1.00000000334148</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>4.33</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>0.23318546400000001</v>
+      </c>
+      <c r="B30" s="1">
+        <v>3.2707331868241001E-12</v>
+      </c>
+      <c r="C30">
+        <v>21737.713414144298</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1.0304465510091299E-8</v>
+      </c>
+      <c r="E30">
+        <v>1.0000000061939101</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>4.34</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>0.24934909999999999</v>
+      </c>
+      <c r="B31" s="1">
+        <v>7.7250329784779794E-12</v>
+      </c>
+      <c r="C31">
+        <v>30024.5896903223</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1.8193841160615201E-8</v>
+      </c>
+      <c r="E31">
+        <v>1.00000000979298</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>0.23295929100000001</v>
+      </c>
+      <c r="B32" s="1">
+        <v>2.5642536500718699E-11</v>
+      </c>
+      <c r="C32">
+        <v>52234.372829619002</v>
+      </c>
+      <c r="D32" s="1">
+        <v>4.41982759795736E-8</v>
+      </c>
+      <c r="E32">
+        <v>1.00000002461008</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>4.72</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>0.25826441100000003</v>
+      </c>
+      <c r="B33" s="1">
+        <v>4.4257791641355102E-12</v>
+      </c>
+      <c r="C33">
+        <v>63958.776051795903</v>
+      </c>
+      <c r="D33" s="1">
+        <v>3.58366534477694E-8</v>
+      </c>
+      <c r="E33">
+        <v>1.00000001968782</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>0.198892347</v>
+      </c>
+      <c r="B34" s="1">
+        <v>6.6100429734205601E-12</v>
+      </c>
+      <c r="C34">
+        <v>71005.201663943793</v>
+      </c>
+      <c r="D34" s="1">
+        <v>6.9339387394869605E-8</v>
+      </c>
+      <c r="E34">
+        <v>1.0000000374732201</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>0.24979715899999999</v>
+      </c>
+      <c r="B35" s="1">
+        <v>7.2105577099038502E-12</v>
+      </c>
+      <c r="C35">
+        <v>112752.614458777</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1.6645780516358099E-7</v>
+      </c>
+      <c r="E35">
+        <v>1.00000008800766</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>5.05</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>0.22719146700000001</v>
+      </c>
+      <c r="B36" s="1">
+        <v>6.1761866526429897E-12</v>
+      </c>
+      <c r="C36">
+        <v>122547.35752634901</v>
+      </c>
+      <c r="D36" s="1">
+        <v>3.41671159124833E-7</v>
+      </c>
+      <c r="E36">
+        <v>1.0000002129501799</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>5.09</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>0.23457409799999901</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1.17024934522028E-11</v>
+      </c>
+      <c r="C37">
+        <v>142366.572343796</v>
+      </c>
+      <c r="D37" s="1">
+        <v>2.8448683589433098E-7</v>
+      </c>
+      <c r="E37">
+        <v>1.00000014790055</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>5.15</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>0.23827221100000001</v>
+      </c>
+      <c r="B38" s="1">
+        <v>5.1498337901994202E-12</v>
+      </c>
+      <c r="C38">
+        <v>171479.57293006001</v>
+      </c>
+      <c r="D38" s="1">
+        <v>3.42753545869431E-7</v>
+      </c>
+      <c r="E38">
+        <v>1.00000020835407</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>5.23</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>0.20758469700000001</v>
+      </c>
+      <c r="B39" s="1">
+        <v>3.4238643300091001E-11</v>
+      </c>
+      <c r="C39">
+        <v>206669.22440523101</v>
+      </c>
+      <c r="D39" s="1">
+        <v>6.2700583729135899E-7</v>
+      </c>
+      <c r="E39">
+        <v>1.0000003154372601</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>5.32</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>0.22299191399999899</v>
+      </c>
+      <c r="B40" s="1">
+        <v>5.3598778762556896E-12</v>
+      </c>
+      <c r="C40">
+        <v>234275.67348778999</v>
+      </c>
+      <c r="D40" s="1">
+        <v>5.4303206350321198E-7</v>
+      </c>
+      <c r="E40">
+        <v>1.0000002651437201</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="0"/>
+        <v>5.37</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>0.239393561999999</v>
+      </c>
+      <c r="B41" s="1">
+        <v>9.4210255945539905E-12</v>
+      </c>
+      <c r="C41">
+        <v>235007.54273043401</v>
+      </c>
+      <c r="D41" s="1">
+        <v>9.76652900437315E-7</v>
+      </c>
+      <c r="E41">
+        <v>1.00000055534004</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="0"/>
+        <v>5.37</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>0.22672709199999999</v>
+      </c>
+      <c r="B42" s="1">
+        <v>6.94428145388583E-12</v>
+      </c>
+      <c r="C42">
+        <v>247435.69337720599</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1.63411955012026E-6</v>
+      </c>
+      <c r="E42">
+        <v>1.0000009077249601</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="0"/>
+        <v>5.39</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>0.24227172299999999</v>
+      </c>
+      <c r="B43" s="1">
+        <v>8.1635328395258203E-12</v>
+      </c>
+      <c r="C43">
+        <v>248208.217547896</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1.15255939101738E-6</v>
+      </c>
+      <c r="E43">
+        <v>1.0000006691671099</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="0"/>
+        <v>5.39</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>0.230606227</v>
+      </c>
+      <c r="B44" s="1">
+        <v>9.7219594082047996E-12</v>
+      </c>
+      <c r="C44">
+        <v>249747.46149905</v>
+      </c>
+      <c r="D44" s="1">
+        <v>8.9128278664490502E-7</v>
+      </c>
+      <c r="E44">
+        <v>1.00000053556658</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="0"/>
+        <v>5.4</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>0.273288949</v>
+      </c>
+      <c r="B45" s="1">
+        <v>1.23450660984761E-11</v>
+      </c>
+      <c r="C45">
+        <v>290825.20485828299</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1.6659175050738601E-6</v>
+      </c>
+      <c r="E45">
+        <v>1.0000008775245</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="0"/>
+        <v>5.46</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>0.21286134599999901</v>
+      </c>
+      <c r="B46" s="1">
+        <v>1.7583556460613001E-12</v>
+      </c>
+      <c r="C46">
+        <v>417161.57636466098</v>
+      </c>
+      <c r="D46" s="1">
+        <v>4.5703167171308696E-6</v>
+      </c>
+      <c r="E46">
+        <v>1.00000293330173</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="0"/>
+        <v>5.62</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>0.23545097400000001</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1.22416787012605E-11</v>
+      </c>
+      <c r="C47">
+        <v>613798.81362835201</v>
+      </c>
+      <c r="D47" s="1">
+        <v>5.1646962745867801E-6</v>
+      </c>
+      <c r="E47">
+        <v>1.00000287825241</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="0"/>
+        <v>5.79</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>0.24532226700000001</v>
+      </c>
+      <c r="B48" s="1">
+        <v>8.2549130814983101E-10</v>
+      </c>
+      <c r="C48">
+        <v>626997.79101573303</v>
+      </c>
+      <c r="D48" s="1">
+        <v>9.7061479941927503E-6</v>
+      </c>
+      <c r="E48">
+        <v>1.00000606341402</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="0"/>
+        <v>5.8</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>0.26731343099999999</v>
+      </c>
+      <c r="B49" s="1">
+        <v>9.6609728760479496E-12</v>
+      </c>
+      <c r="C49">
+        <v>801306.22353820805</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1.39005887566621E-5</v>
+      </c>
+      <c r="E49">
+        <v>1.0000074980576401</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="0"/>
+        <v>5.9</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>0.27074934099999998</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1.56715316194014E-11</v>
+      </c>
+      <c r="C50">
+        <v>987196.43609744206</v>
+      </c>
+      <c r="D50" s="1">
+        <v>9.6324109557660993E-6</v>
+      </c>
+      <c r="E50">
+        <v>1.00000442023224</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="0"/>
+        <v>5.99</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>0.23728226999999999</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1.35697588237962E-11</v>
+      </c>
+      <c r="C51">
+        <v>1830489.8458953099</v>
+      </c>
+      <c r="D51" s="1">
+        <v>6.5556500924690895E-5</v>
+      </c>
+      <c r="E51">
+        <v>1.0000346211021001</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="0"/>
+        <v>6.26</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>0.24682641</v>
+      </c>
+      <c r="B52" s="1">
+        <v>2.3307663900911699E-11</v>
+      </c>
+      <c r="C52">
+        <v>3409665.3936576098</v>
+      </c>
+      <c r="D52">
+        <v>1.17896892799889E-4</v>
+      </c>
+      <c r="E52">
+        <v>1.0000608559340101</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="0"/>
+        <v>6.53</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>0.22176915899999999</v>
+      </c>
+      <c r="B53" s="1">
+        <v>2.04201828464704E-11</v>
+      </c>
+      <c r="C53">
+        <v>3931111.45281384</v>
+      </c>
+      <c r="D53">
+        <v>2.7594106146435198E-4</v>
+      </c>
+      <c r="E53">
+        <v>1.0001544361239401</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="0"/>
+        <v>6.59</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>0.27577460199999998</v>
+      </c>
+      <c r="B54" s="1">
+        <v>1.0640085345802099E-11</v>
+      </c>
+      <c r="C54">
+        <v>4711597.0502990102</v>
+      </c>
+      <c r="D54">
+        <v>3.3162254451017399E-4</v>
+      </c>
+      <c r="E54">
+        <v>1.00016106062113</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="0"/>
+        <v>6.67</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>0.24865711700000001</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1.9468958106471801E-11</v>
+      </c>
+      <c r="C55">
+        <v>4850120.4055153597</v>
+      </c>
+      <c r="D55">
+        <v>2.7923402991196798E-4</v>
+      </c>
+      <c r="E55">
+        <v>1.0001568319337599</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="0"/>
+        <v>6.69</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>0.26441577799999999</v>
+      </c>
+      <c r="B56" s="1">
+        <v>6.1497912989028598E-11</v>
+      </c>
+      <c r="C56">
+        <v>4908879.8723105099</v>
+      </c>
+      <c r="D56">
+        <v>4.3573436023951998E-4</v>
+      </c>
+      <c r="E56">
+        <v>1.00023166427938</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="0"/>
+        <v>6.69</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>0.25109600900000001</v>
+      </c>
+      <c r="B57" s="1">
+        <v>2.1291470229005499E-11</v>
+      </c>
+      <c r="C57">
+        <v>18820088.454929199</v>
+      </c>
+      <c r="D57">
+        <v>5.2229690322284804E-3</v>
+      </c>
+      <c r="E57">
+        <v>1.00270162743997</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="0"/>
+        <v>7.27</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>0.27936535000000001</v>
+      </c>
+      <c r="B58" s="1">
+        <v>9.8281373220769096E-11</v>
+      </c>
+      <c r="C58">
+        <v>19929150.650849201</v>
+      </c>
+      <c r="D58">
+        <v>6.5221627936442499E-3</v>
+      </c>
+      <c r="E58">
+        <v>1.00332373184797</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="0"/>
+        <v>7.3</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>0.22793823299999999</v>
+      </c>
+      <c r="B59" s="1">
+        <v>3.8148168996315904E-9</v>
+      </c>
+      <c r="C59">
+        <v>29956878.443828199</v>
+      </c>
+      <c r="D59">
+        <v>1.7711339070871399E-2</v>
+      </c>
+      <c r="E59">
+        <v>1.0114170674742999</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="0"/>
+        <v>7.48</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="1"/>
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>0.26706729099999998</v>
+      </c>
+      <c r="B60" s="1">
+        <v>2.8513653892117101E-11</v>
+      </c>
+      <c r="C60">
+        <v>33562178.7262372</v>
+      </c>
+      <c r="D60">
+        <v>1.0303406763810599E-2</v>
+      </c>
+      <c r="E60">
+        <v>1.0055544942982</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="0"/>
+        <v>7.53</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="1"/>
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>0.24099679500000001</v>
+      </c>
+      <c r="B61" s="1">
+        <v>9.1616626454163102E-12</v>
+      </c>
+      <c r="C61">
+        <v>34731106.939295404</v>
+      </c>
+      <c r="D61">
+        <v>2.55563378501081E-2</v>
+      </c>
+      <c r="E61">
+        <v>1.0135107727763999</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="0"/>
+        <v>7.54</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="1"/>
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>0.28398292600000002</v>
+      </c>
+      <c r="B62" s="1">
+        <v>1.26992219800946E-11</v>
+      </c>
+      <c r="C62">
+        <v>35902589.158120804</v>
+      </c>
+      <c r="D62">
+        <v>2.3199663432142099E-2</v>
+      </c>
+      <c r="E62">
+        <v>1.01136131536005</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="0"/>
+        <v>7.56</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="1"/>
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>0.22188668</v>
+      </c>
+      <c r="B63" s="1">
+        <v>2.71343334139877E-11</v>
+      </c>
+      <c r="C63">
+        <v>39436969.062866896</v>
+      </c>
+      <c r="D63">
+        <v>2.98721365239519E-2</v>
+      </c>
+      <c r="E63">
+        <v>1.0158501755717799</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="0"/>
+        <v>7.6</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="1"/>
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>0.255069606</v>
+      </c>
+      <c r="B64" s="1">
+        <v>1.4917353322030701E-11</v>
+      </c>
+      <c r="C64">
+        <v>41951457.395388901</v>
+      </c>
+      <c r="D64">
+        <v>2.3674618203118301E-2</v>
+      </c>
+      <c r="E64">
+        <v>1.01254833865705</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="0"/>
+        <v>7.62</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="1"/>
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>0.25913322699999902</v>
+      </c>
+      <c r="B65" s="1">
+        <v>1.7292197809425999E-11</v>
+      </c>
+      <c r="C65">
+        <v>58705818.287478402</v>
+      </c>
+      <c r="D65">
+        <v>5.25481455819065E-2</v>
+      </c>
+      <c r="E65">
+        <v>1.0295119380334901</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="0"/>
+        <v>7.77</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="1"/>
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>0.271544375</v>
+      </c>
+      <c r="B66" s="1">
+        <v>3.8784590188924201E-11</v>
+      </c>
+      <c r="C66">
+        <v>68434738.422273606</v>
+      </c>
+      <c r="D66">
+        <v>9.2310852978572902E-2</v>
+      </c>
+      <c r="E66">
+        <v>1.05474047314153</v>
+      </c>
+      <c r="G66">
+        <f t="shared" ref="G66:G72" si="2">ROUND(LOG10(C66),2)</f>
+        <v>7.84</v>
+      </c>
+      <c r="H66">
+        <f t="shared" ref="H66:H72" si="3">ROUND(E66,2)</f>
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>0.28155577900000001</v>
+      </c>
+      <c r="B67" s="1">
+        <v>5.5462195931140202E-11</v>
+      </c>
+      <c r="C67">
+        <v>84872099.063106194</v>
+      </c>
+      <c r="D67">
+        <v>8.6779320067369103E-2</v>
+      </c>
+      <c r="E67">
+        <v>1.04671495910248</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="2"/>
+        <v>7.93</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="3"/>
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>0.28170716099999998</v>
+      </c>
+      <c r="B68" s="1">
+        <v>1.4682394119382001E-10</v>
+      </c>
+      <c r="C68">
+        <v>122920158.745252</v>
+      </c>
+      <c r="D68">
+        <v>0.247042999793745</v>
+      </c>
+      <c r="E68">
+        <v>1.1326427985054699</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="2"/>
+        <v>8.09</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="3"/>
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>0.28307722800000001</v>
+      </c>
+      <c r="B69" s="1">
+        <v>2.0580406650891599E-11</v>
+      </c>
+      <c r="C69">
+        <v>158599499.74315101</v>
+      </c>
+      <c r="D69">
+        <v>0.49106513079666803</v>
+      </c>
+      <c r="E69">
+        <v>1.2601972367001999</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="2"/>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="3"/>
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>0.25236639700000002</v>
+      </c>
+      <c r="B70" s="1">
+        <v>1.19708144388057E-11</v>
+      </c>
+      <c r="C70">
+        <v>191746036.81893799</v>
+      </c>
+      <c r="D70">
+        <v>1.4220512781316299</v>
+      </c>
+      <c r="E70">
+        <v>1.73434715633852</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="2"/>
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="3"/>
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>0.253408352</v>
+      </c>
+      <c r="B71" s="1">
+        <v>5.266296543459E-11</v>
+      </c>
+      <c r="C71">
+        <v>206669229.357602</v>
+      </c>
+      <c r="D71">
+        <v>0.82645793547409796</v>
+      </c>
+      <c r="E71">
+        <v>1.51693072258017</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="2"/>
+        <v>8.32</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="3"/>
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>0.27746309499999999</v>
+      </c>
+      <c r="B72" s="1">
+        <v>8.1732362710988004E-11</v>
+      </c>
+      <c r="C72">
+        <v>266415609.008506</v>
+      </c>
+      <c r="D72">
+        <v>3.3948104187538002</v>
+      </c>
+      <c r="E72">
+        <v>2.5011943485015502</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="2"/>
+        <v>8.43</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="3"/>
+        <v>2.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:E72">
+    <sortCondition ref="C1:C72"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>